<commit_message>
Added test case 008
</commit_message>
<xml_diff>
--- a/orangeHRM-TESTCASES.xlsx
+++ b/orangeHRM-TESTCASES.xlsx
@@ -1224,7 +1224,7 @@
       <name val="Open Sans"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1261,8 +1261,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1294,11 +1300,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1364,6 +1383,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2457,8 +2488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2722,65 +2753,68 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="111.75" customHeight="1">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="23" t="s">
+      <c r="B8" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="26" t="s">
         <v>274</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="26" t="s">
         <v>275</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="26" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="125.25" customHeight="1">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:11" s="15" customFormat="1" ht="125.25" customHeight="1">
+      <c r="A9" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="29" t="s">
         <v>111</v>
       </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
     </row>
     <row r="10" spans="1:11" ht="69.75" customHeight="1">
       <c r="A10" s="1" t="s">

</xml_diff>

<commit_message>
Implemented Test cases 9 and 10
</commit_message>
<xml_diff>
--- a/orangeHRM-TESTCASES.xlsx
+++ b/orangeHRM-TESTCASES.xlsx
@@ -1224,7 +1224,7 @@
       <name val="Open Sans"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1264,6 +1264,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1317,7 +1323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1381,9 +1387,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1395,6 +1398,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2488,8 +2505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2753,120 +2770,126 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="111.75" customHeight="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="26" t="s">
+      <c r="B8" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="I8" s="25" t="s">
         <v>274</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="25" t="s">
         <v>275</v>
       </c>
-      <c r="K8" s="26" t="s">
+      <c r="K8" s="25" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="15" customFormat="1" ht="125.25" customHeight="1">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:11" s="34" customFormat="1" ht="125.25" customHeight="1">
+      <c r="A9" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="28" t="s">
+      <c r="B9" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-    </row>
-    <row r="10" spans="1:11" ht="69.75" customHeight="1">
-      <c r="A10" s="1" t="s">
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+    </row>
+    <row r="10" spans="1:11" s="30" customFormat="1" ht="69.75" customHeight="1">
+      <c r="A10" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="28" t="s">
         <v>115</v>
       </c>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" ht="142.5" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="28" t="s">
         <v>118</v>
       </c>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" ht="175.5" customHeight="1">
       <c r="A12" s="1" t="s">
@@ -3795,7 +3818,7 @@
       <c r="B2" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="29">
         <v>7</v>
       </c>
     </row>
@@ -3806,7 +3829,7 @@
       <c r="B3" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="25"/>
+      <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="14" t="s">
@@ -3815,7 +3838,7 @@
       <c r="B4" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="25"/>
+      <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="16" t="s">
@@ -3824,7 +3847,7 @@
       <c r="B5" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="25"/>
+      <c r="C5" s="29"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="16" t="s">
@@ -3833,7 +3856,7 @@
       <c r="B6" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="25"/>
+      <c r="C6" s="29"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="16" t="s">
@@ -3842,7 +3865,7 @@
       <c r="B7" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="16" t="s">
@@ -3851,7 +3874,7 @@
       <c r="B8" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="25"/>
+      <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="14" t="s">
@@ -3860,7 +3883,7 @@
       <c r="B9" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="25"/>
+      <c r="C9" s="29"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="16" t="s">
@@ -3869,7 +3892,7 @@
       <c r="B10" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="25"/>
+      <c r="C10" s="29"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="14" t="s">
@@ -3878,7 +3901,7 @@
       <c r="B11" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="29"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="16" t="s">
@@ -3887,7 +3910,7 @@
       <c r="B12" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="29">
         <v>3</v>
       </c>
     </row>
@@ -3898,7 +3921,7 @@
       <c r="B13" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="29"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="16" t="s">
@@ -3907,7 +3930,7 @@
       <c r="B14" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="25"/>
+      <c r="C14" s="29"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="14" t="s">
@@ -3916,7 +3939,7 @@
       <c r="B15" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="29">
         <v>3</v>
       </c>
     </row>
@@ -3927,7 +3950,7 @@
       <c r="B16" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="C16" s="25"/>
+      <c r="C16" s="29"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="14" t="s">
@@ -3936,7 +3959,7 @@
       <c r="B17" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="C17" s="25"/>
+      <c r="C17" s="29"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="16" t="s">
@@ -3945,7 +3968,7 @@
       <c r="B18" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="29">
         <v>4</v>
       </c>
     </row>
@@ -3956,7 +3979,7 @@
       <c r="B19" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C19" s="25"/>
+      <c r="C19" s="29"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="16" t="s">
@@ -3965,7 +3988,7 @@
       <c r="B20" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="C20" s="25"/>
+      <c r="C20" s="29"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="14" t="s">
@@ -3974,7 +3997,7 @@
       <c r="B21" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="C21" s="25"/>
+      <c r="C21" s="29"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="16" t="s">
@@ -4016,7 +4039,7 @@
       <c r="B25" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="C25" s="25">
+      <c r="C25" s="29">
         <v>18</v>
       </c>
     </row>
@@ -4027,7 +4050,7 @@
       <c r="B26" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="C26" s="25"/>
+      <c r="C26" s="29"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="14" t="s">
@@ -4036,7 +4059,7 @@
       <c r="B27" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="C27" s="25"/>
+      <c r="C27" s="29"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="16" t="s">
@@ -4045,7 +4068,7 @@
       <c r="B28" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="C28" s="25"/>
+      <c r="C28" s="29"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="14" t="s">
@@ -4054,7 +4077,7 @@
       <c r="B29" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="C29" s="25"/>
+      <c r="C29" s="29"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="16" t="s">
@@ -4063,7 +4086,7 @@
       <c r="B30" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="C30" s="25"/>
+      <c r="C30" s="29"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="14" t="s">
@@ -4072,7 +4095,7 @@
       <c r="B31" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="C31" s="25"/>
+      <c r="C31" s="29"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="16" t="s">
@@ -4081,7 +4104,7 @@
       <c r="B32" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="C32" s="25"/>
+      <c r="C32" s="29"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="14" t="s">
@@ -4090,7 +4113,7 @@
       <c r="B33" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="C33" s="25"/>
+      <c r="C33" s="29"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="16" t="s">
@@ -4099,7 +4122,7 @@
       <c r="B34" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="C34" s="25"/>
+      <c r="C34" s="29"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="14" t="s">
@@ -4108,7 +4131,7 @@
       <c r="B35" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="C35" s="25"/>
+      <c r="C35" s="29"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="16" t="s">
@@ -4117,7 +4140,7 @@
       <c r="B36" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="C36" s="25"/>
+      <c r="C36" s="29"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="14" t="s">
@@ -4126,7 +4149,7 @@
       <c r="B37" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="C37" s="25"/>
+      <c r="C37" s="29"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="16" t="s">
@@ -4135,7 +4158,7 @@
       <c r="B38" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="C38" s="25"/>
+      <c r="C38" s="29"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="14" t="s">
@@ -4144,7 +4167,7 @@
       <c r="B39" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="C39" s="25"/>
+      <c r="C39" s="29"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="16" t="s">
@@ -4153,7 +4176,7 @@
       <c r="B40" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="C40" s="25"/>
+      <c r="C40" s="29"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="14" t="s">
@@ -4162,7 +4185,7 @@
       <c r="B41" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="C41" s="25"/>
+      <c r="C41" s="29"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="16" t="s">
@@ -4171,7 +4194,7 @@
       <c r="B42" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="C42" s="25"/>
+      <c r="C42" s="29"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="14" t="s">
@@ -4180,7 +4203,7 @@
       <c r="B43" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="C43" s="25">
+      <c r="C43" s="29">
         <v>4</v>
       </c>
     </row>
@@ -4191,7 +4214,7 @@
       <c r="B44" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="C44" s="25"/>
+      <c r="C44" s="29"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="14" t="s">
@@ -4200,7 +4223,7 @@
       <c r="B45" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="C45" s="25"/>
+      <c r="C45" s="29"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="16" t="s">
@@ -4209,7 +4232,7 @@
       <c r="B46" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="C46" s="25"/>
+      <c r="C46" s="29"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="20"/>

</xml_diff>